<commit_message>
Adding weighted survey results
</commit_message>
<xml_diff>
--- a/2015-call-for-speakers/SurveySummary-Weighted.xlsx
+++ b/2015-call-for-speakers/SurveySummary-Weighted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="90" windowWidth="29925" windowHeight="15000" activeTab="1"/>
+    <workbookView xWindow="8460" yWindow="90" windowWidth="25440" windowHeight="15000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -848,82 +848,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -937,214 +862,7 @@
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1154,6 +872,250 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[SurveySummary-Weighted.xlsx]Pivoted!PivotTable1</c:name>
+    <c:fmtId val="11"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pivoted!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Pivoted!$F$4:$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Big Data &amp; NoSQL Technology</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Professional Development</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Reporting and Information Delivery</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Business Intelligence</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Application and Database Development</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Enterprise Database Administration &amp; Deployment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pivoted!$G$4:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2414404761904798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.79090476190476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4019047619047602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7929047619047598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3788809523809502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5658690476190502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="195779968"/>
+        <c:axId val="195728512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="195779968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="195728512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="195728512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="195779968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2003,7 +1965,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="F3:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisPage" showAll="0">
@@ -2192,7 +2154,7 @@
     <dataField name="Average of Average" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="43"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="39">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2201,14 +2163,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="2">
+  <chartFormats count="4">
     <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -2219,6 +2181,24 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="10" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2375,8 +2355,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Category"/>
     <tableColumn id="2" name="Question"/>
-    <tableColumn id="3" name="Sum" dataDxfId="97" dataCellStyle="Comma"/>
-    <tableColumn id="4" name="Average" dataDxfId="98" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Sum" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="Average" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2637,7 +2617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -17337,8 +17317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19111,8 +19091,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>